<commit_message>
Add/Remove from favorites updated
</commit_message>
<xml_diff>
--- a/login_credentials.xlsx
+++ b/login_credentials.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasha\IdeaProjects\HomeWorks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c9a0b6844abb40dc/Desktop/Java/trycloud/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C67238D-8518-4F5E-A5C9-D212A743D531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{1C67238D-8518-4F5E-A5C9-D212A743D531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70FE1B43-4F1E-4D21-8FAF-B916539DF861}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CCBB5B2E-1A4F-460D-9020-42FC3957DA31}"/>
+    <workbookView xWindow="2904" yWindow="1656" windowWidth="17280" windowHeight="8880" xr2:uid="{CCBB5B2E-1A4F-460D-9020-42FC3957DA31}"/>
   </bookViews>
   <sheets>
     <sheet name="credentials" sheetId="1" r:id="rId1"/>
@@ -423,11 +423,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89769708-668A-4A82-8FC5-FCDFD629835A}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -479,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689B8475-609B-4F01-A0A5-5638C24B4C7A}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>

</xml_diff>